<commit_message>
Health and elemental mechanic now being used
</commit_message>
<xml_diff>
--- a/Documentation/Weakness Chart.xlsx
+++ b/Documentation/Weakness Chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Blue</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Fire</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
   <dimension ref="E3:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,26 +451,29 @@
     </row>
     <row r="10" spans="5:9">
       <c r="F10" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="5:9">
       <c r="E11" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
@@ -473,7 +482,7 @@
     </row>
     <row r="12" spans="5:9">
       <c r="E12" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -490,7 +499,7 @@
     </row>
     <row r="13" spans="5:9">
       <c r="E13" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -507,7 +516,7 @@
     </row>
     <row r="14" spans="5:9">
       <c r="E14" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <v>0</v>

</xml_diff>